<commit_message>
scarcity model new simulation runs
</commit_message>
<xml_diff>
--- a/Mathematical Model/Scarcity Model/parameters_w_50/ alpha/NonEmpty_diff_alpha1_firstrun.xlsx
+++ b/Mathematical Model/Scarcity Model/parameters_w_50/ alpha/NonEmpty_diff_alpha1_firstrun.xlsx
@@ -452,25 +452,25 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5434782608695652</v>
+        <v>0.5490196078431373</v>
       </c>
       <c r="C3">
-        <v>0.5010893246187363</v>
+        <v>0.5056689342403629</v>
       </c>
       <c r="D3">
-        <v>0.4853556485355648</v>
+        <v>0.5433962264150943</v>
       </c>
       <c r="E3">
-        <v>0.5053533190578159</v>
+        <v>0.5032967032967033</v>
       </c>
       <c r="F3">
-        <v>0.5062761506276151</v>
+        <v>0.5021097046413502</v>
       </c>
       <c r="G3">
-        <v>0.4926931106471816</v>
+        <v>0.4947145877378435</v>
       </c>
       <c r="H3">
-        <v>0.504</v>
+        <v>0.494</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -478,25 +478,25 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.5679012345679012</v>
+        <v>0.4794520547945205</v>
       </c>
       <c r="C4">
-        <v>0.5021834061135371</v>
+        <v>0.5138248847926268</v>
       </c>
       <c r="D4">
-        <v>0.4868421052631579</v>
+        <v>0.5449438202247191</v>
       </c>
       <c r="E4">
-        <v>0.5168374816983895</v>
+        <v>0.4876160990712075</v>
       </c>
       <c r="F4">
-        <v>0.4324324324324325</v>
+        <v>0.4733333333333333</v>
       </c>
       <c r="G4">
-        <v>0.4957865168539326</v>
+        <v>0.4964234620886981</v>
       </c>
       <c r="H4">
-        <v>0.494</v>
+        <v>0.504</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -504,25 +504,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5057471264367817</v>
+        <v>0.4933333333333333</v>
       </c>
       <c r="C5">
-        <v>0.5021097046413502</v>
+        <v>0.5183585313174947</v>
       </c>
       <c r="D5">
-        <v>0.5161290322580645</v>
+        <v>0.4957264957264957</v>
       </c>
       <c r="E5">
-        <v>0.5105263157894737</v>
+        <v>0.4904891304347826</v>
       </c>
       <c r="F5">
-        <v>0.39</v>
+        <v>0.462962962962963</v>
       </c>
       <c r="G5">
-        <v>0.5127226463104325</v>
+        <v>0.5095541401273885</v>
       </c>
       <c r="H5">
-        <v>0.492</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -530,25 +530,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.4659090909090909</v>
+        <v>0.4691358024691358</v>
       </c>
       <c r="C6">
-        <v>0.5077821011673151</v>
+        <v>0.515748031496063</v>
       </c>
       <c r="D6">
-        <v>0.3928571428571428</v>
+        <v>0.4905660377358491</v>
       </c>
       <c r="E6">
-        <v>0.5057179161372299</v>
+        <v>0.5</v>
       </c>
       <c r="F6">
-        <v>0.4639175257731959</v>
+        <v>0.5</v>
       </c>
       <c r="G6">
-        <v>0.5091352009744214</v>
+        <v>0.5135802469135803</v>
       </c>
       <c r="H6">
-        <v>0.486</v>
+        <v>0.474</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -556,25 +556,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.4653465346534654</v>
+        <v>0.4623655913978494</v>
       </c>
       <c r="C7">
-        <v>0.5118829981718465</v>
+        <v>0.5268022181146026</v>
       </c>
       <c r="D7">
-        <v>0.4299065420560748</v>
+        <v>0.4565217391304348</v>
       </c>
       <c r="E7">
-        <v>0.520460358056266</v>
+        <v>0.5050761421319797</v>
       </c>
       <c r="F7">
-        <v>0.4545454545454545</v>
+        <v>0.4301075268817204</v>
       </c>
       <c r="G7">
-        <v>0.5074257425742574</v>
+        <v>0.5116564417177915</v>
       </c>
       <c r="H7">
-        <v>0.474</v>
+        <v>0.468</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -582,25 +582,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.4513274336283186</v>
+        <v>0.4259259259259259</v>
       </c>
       <c r="C8">
-        <v>0.5139372822299652</v>
+        <v>0.5266781411359724</v>
       </c>
       <c r="D8">
-        <v>0.4414414414414414</v>
+        <v>0.4571428571428571</v>
       </c>
       <c r="E8">
-        <v>0.5103092783505154</v>
+        <v>0.5074812967581047</v>
       </c>
       <c r="F8">
-        <v>0.4421052631578947</v>
+        <v>0.47</v>
       </c>
       <c r="G8">
-        <v>0.5012315270935961</v>
+        <v>0.5092707045735476</v>
       </c>
       <c r="H8">
-        <v>0.464</v>
+        <v>0.478</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -608,25 +608,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.4646464646464646</v>
+        <v>0.4193548387096774</v>
       </c>
       <c r="C9">
-        <v>0.5182724252491694</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="D9">
-        <v>0.4661016949152542</v>
+        <v>0.5425531914893617</v>
       </c>
       <c r="E9">
-        <v>0.5096774193548387</v>
+        <v>0.5063291139240507</v>
       </c>
       <c r="F9">
-        <v>0.4387755102040816</v>
+        <v>0.4489795918367347</v>
       </c>
       <c r="G9">
-        <v>0.5</v>
+        <v>0.5012468827930174</v>
       </c>
       <c r="H9">
-        <v>0.466</v>
+        <v>0.484</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -634,25 +634,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.4705882352941176</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="C10">
-        <v>0.512781954887218</v>
+        <v>0.545045045045045</v>
       </c>
       <c r="D10">
-        <v>0.4369747899159664</v>
+        <v>0.4607843137254902</v>
       </c>
       <c r="E10">
-        <v>0.5103092783505154</v>
+        <v>0.5037688442211056</v>
       </c>
       <c r="F10">
-        <v>0.404040404040404</v>
+        <v>0.4247787610619469</v>
       </c>
       <c r="G10">
-        <v>0.5006180469715699</v>
+        <v>0.5006257822277848</v>
       </c>
       <c r="H10">
-        <v>0.452</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -660,25 +660,25 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.4606741573033708</v>
+        <v>0.4814814814814815</v>
       </c>
       <c r="C11">
-        <v>0.5109489051094891</v>
+        <v>0.546875</v>
       </c>
       <c r="D11">
-        <v>0.3909090909090909</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="E11">
-        <v>0.5173745173745173</v>
+        <v>0.4975</v>
       </c>
       <c r="F11">
-        <v>0.4021739130434783</v>
+        <v>0.3942307692307692</v>
       </c>
       <c r="G11">
-        <v>0.4932349323493235</v>
+        <v>0.4955974842767296</v>
       </c>
       <c r="H11">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -686,25 +686,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.4479166666666667</v>
+        <v>0.4672897196261682</v>
       </c>
       <c r="C12">
-        <v>0.5093833780160858</v>
+        <v>0.5380507343124166</v>
       </c>
       <c r="D12">
-        <v>0.4234234234234234</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E12">
-        <v>0.5226390685640362</v>
+        <v>0.4981226533166458</v>
       </c>
       <c r="F12">
-        <v>0.367816091954023</v>
+        <v>0.5154639175257731</v>
       </c>
       <c r="G12">
-        <v>0.4919254658385093</v>
+        <v>0.4901234567901235</v>
       </c>
       <c r="H12">
-        <v>0.462</v>
+        <v>0.488</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -712,25 +712,25 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.47</v>
+        <v>0.5673076923076923</v>
       </c>
       <c r="C13">
-        <v>0.5127877237851662</v>
+        <v>0.5455712451861361</v>
       </c>
       <c r="D13">
-        <v>0.4666666666666667</v>
+        <v>0.4326923076923077</v>
       </c>
       <c r="E13">
-        <v>0.517464424320828</v>
+        <v>0.5044359949302915</v>
       </c>
       <c r="F13">
-        <v>0.4134615384615384</v>
+        <v>0.4252873563218391</v>
       </c>
       <c r="G13">
-        <v>0.4944375772558715</v>
+        <v>0.4775</v>
       </c>
       <c r="H13">
-        <v>0.452</v>
+        <v>0.494</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -738,25 +738,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.4615384615384616</v>
+        <v>0.5242718446601942</v>
       </c>
       <c r="C14">
-        <v>0.5138387484957883</v>
+        <v>0.5273390036452005</v>
       </c>
       <c r="D14">
-        <v>0.5041322314049587</v>
+        <v>0.425</v>
       </c>
       <c r="E14">
-        <v>0.5102301790281329</v>
+        <v>0.5135135135135135</v>
       </c>
       <c r="F14">
-        <v>0.4242424242424243</v>
+        <v>0.3457943925233645</v>
       </c>
       <c r="G14">
-        <v>0.4900744416873449</v>
+        <v>0.489414694894147</v>
       </c>
       <c r="H14">
-        <v>0.446</v>
+        <v>0.476</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -764,25 +764,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.4272727272727272</v>
+        <v>0.4857142857142857</v>
       </c>
       <c r="C15">
-        <v>0.5137931034482759</v>
+        <v>0.5348837209302325</v>
       </c>
       <c r="D15">
-        <v>0.4245283018867925</v>
+        <v>0.4690265486725664</v>
       </c>
       <c r="E15">
-        <v>0.5006385696040868</v>
+        <v>0.5071707953063885</v>
       </c>
       <c r="F15">
-        <v>0.4623655913978494</v>
+        <v>0.3423423423423423</v>
       </c>
       <c r="G15">
-        <v>0.4876543209876543</v>
+        <v>0.4917617237008872</v>
       </c>
       <c r="H15">
-        <v>0.438</v>
+        <v>0.476</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -790,25 +790,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.4150943396226415</v>
+        <v>0.4824561403508772</v>
       </c>
       <c r="C16">
-        <v>0.5142231947483589</v>
+        <v>0.5398230088495575</v>
       </c>
       <c r="D16">
-        <v>0.4504504504504505</v>
+        <v>0.4453781512605042</v>
       </c>
       <c r="E16">
-        <v>0.5031525851197982</v>
+        <v>0.4936061381074169</v>
       </c>
       <c r="F16">
-        <v>0.5196078431372549</v>
+        <v>0.3826086956521739</v>
       </c>
       <c r="G16">
-        <v>0.4828009828009828</v>
+        <v>0.4855708908406525</v>
       </c>
       <c r="H16">
-        <v>0.444</v>
+        <v>0.482</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -816,25 +816,25 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.4824561403508772</v>
+        <v>0.4434782608695652</v>
       </c>
       <c r="C17">
-        <v>0.5115546218487395</v>
+        <v>0.5395299145299145</v>
       </c>
       <c r="D17">
-        <v>0.5392156862745098</v>
+        <v>0.4476190476190476</v>
       </c>
       <c r="E17">
-        <v>0.5089974293059126</v>
+        <v>0.4974358974358974</v>
       </c>
       <c r="F17">
-        <v>0.5416666666666666</v>
+        <v>0.4175824175824176</v>
       </c>
       <c r="G17">
-        <v>0.4773869346733668</v>
+        <v>0.4805031446540881</v>
       </c>
       <c r="H17">
-        <v>0.442</v>
+        <v>0.472</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -842,25 +842,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.4745762711864407</v>
+        <v>0.4466019417475728</v>
       </c>
       <c r="C18">
-        <v>0.5101832993890021</v>
+        <v>0.5421810699588477</v>
       </c>
       <c r="D18">
-        <v>0.5535714285714286</v>
+        <v>0.5042735042735043</v>
       </c>
       <c r="E18">
-        <v>0.4948586118251928</v>
+        <v>0.4840357598978289</v>
       </c>
       <c r="F18">
-        <v>0.4830508474576271</v>
+        <v>0.4183673469387755</v>
       </c>
       <c r="G18">
-        <v>0.4791929382093317</v>
+        <v>0.4782067247820673</v>
       </c>
       <c r="H18">
-        <v>0.444</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -868,25 +868,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.4615384615384616</v>
+        <v>0.4526315789473684</v>
       </c>
       <c r="C19">
-        <v>0.5184108527131783</v>
+        <v>0.5395894428152492</v>
       </c>
       <c r="D19">
-        <v>0.4745762711864407</v>
+        <v>0.4919354838709677</v>
       </c>
       <c r="E19">
-        <v>0.4930114358322745</v>
+        <v>0.479328165374677</v>
       </c>
       <c r="F19">
-        <v>0.5565217391304348</v>
+        <v>0.514018691588785</v>
       </c>
       <c r="G19">
-        <v>0.485424588086185</v>
+        <v>0.4794007490636704</v>
       </c>
       <c r="H19">
-        <v>0.428</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -894,25 +894,25 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.4521739130434783</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="C20">
-        <v>0.5229615745079662</v>
+        <v>0.5382462686567164</v>
       </c>
       <c r="D20">
-        <v>0.3867924528301887</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="E20">
-        <v>0.4954838709677419</v>
+        <v>0.4896640826873385</v>
       </c>
       <c r="F20">
-        <v>0.5698924731182796</v>
+        <v>0.4432989690721649</v>
       </c>
       <c r="G20">
-        <v>0.4872448979591837</v>
+        <v>0.4756554307116105</v>
       </c>
       <c r="H20">
-        <v>0.428</v>
+        <v>0.472</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -920,25 +920,25 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.4406779661016949</v>
+        <v>0.5104166666666666</v>
       </c>
       <c r="C21">
-        <v>0.5231187669990934</v>
+        <v>0.5377697841726619</v>
       </c>
       <c r="D21">
-        <v>0.4152542372881356</v>
+        <v>0.4504504504504505</v>
       </c>
       <c r="E21">
-        <v>0.4987046632124352</v>
+        <v>0.4923664122137404</v>
       </c>
       <c r="F21">
-        <v>0.5048543689320388</v>
+        <v>0.4148936170212766</v>
       </c>
       <c r="G21">
-        <v>0.4962216624685138</v>
+        <v>0.4764851485148515</v>
       </c>
       <c r="H21">
-        <v>0.424</v>
+        <v>0.472</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -946,25 +946,25 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.4433962264150944</v>
+        <v>0.5145631067961165</v>
       </c>
       <c r="C22">
-        <v>0.5235602094240838</v>
+        <v>0.5337954939341422</v>
       </c>
       <c r="D22">
-        <v>0.4732142857142857</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E22">
-        <v>0.4928848641655886</v>
+        <v>0.4885496183206107</v>
       </c>
       <c r="F22">
-        <v>0.4444444444444444</v>
+        <v>0.4489795918367347</v>
       </c>
       <c r="G22">
-        <v>0.509386733416771</v>
+        <v>0.4753694581280788</v>
       </c>
       <c r="H22">
-        <v>0.414</v>
+        <v>0.482</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -972,25 +972,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.4705882352941176</v>
+        <v>0.4947368421052631</v>
       </c>
       <c r="C23">
-        <v>0.5222502099076406</v>
+        <v>0.5331654072208228</v>
       </c>
       <c r="D23">
-        <v>0.462962962962963</v>
+        <v>0.4591836734693878</v>
       </c>
       <c r="E23">
-        <v>0.4948717948717949</v>
+        <v>0.4778761061946903</v>
       </c>
       <c r="F23">
-        <v>0.42</v>
+        <v>0.4653465346534654</v>
       </c>
       <c r="G23">
-        <v>0.5119798234552333</v>
+        <v>0.4659231722428748</v>
       </c>
       <c r="H23">
-        <v>0.406</v>
+        <v>0.476</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -998,25 +998,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.4672897196261682</v>
+        <v>0.5096153846153846</v>
       </c>
       <c r="C24">
-        <v>0.5182481751824818</v>
+        <v>0.5385239253852393</v>
       </c>
       <c r="D24">
-        <v>0.5135135135135135</v>
+        <v>0.4271844660194175</v>
       </c>
       <c r="E24">
-        <v>0.4961734693877551</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="F24">
-        <v>0.3364485981308411</v>
+        <v>0.53125</v>
       </c>
       <c r="G24">
-        <v>0.5181476846057572</v>
+        <v>0.4654088050314465</v>
       </c>
       <c r="H24">
-        <v>0.404</v>
+        <v>0.466</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1024,25 +1024,25 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.5178571428571429</v>
+        <v>0.4380952380952381</v>
       </c>
       <c r="C25">
-        <v>0.5167464114832536</v>
+        <v>0.5339652448657188</v>
       </c>
       <c r="D25">
-        <v>0.5148514851485149</v>
+        <v>0.3983050847457627</v>
       </c>
       <c r="E25">
-        <v>0.4896907216494845</v>
+        <v>0.4879898862199747</v>
       </c>
       <c r="F25">
-        <v>0.3942307692307692</v>
+        <v>0.392156862745098</v>
       </c>
       <c r="G25">
-        <v>0.5201005025125628</v>
+        <v>0.4708798017348203</v>
       </c>
       <c r="H25">
-        <v>0.406</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1050,25 +1050,25 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.5</v>
+        <v>0.4622641509433962</v>
       </c>
       <c r="C26">
-        <v>0.5179127725856698</v>
+        <v>0.5409961685823754</v>
       </c>
       <c r="D26">
-        <v>0.5</v>
+        <v>0.4528301886792453</v>
       </c>
       <c r="E26">
-        <v>0.4987179487179487</v>
+        <v>0.4910714285714285</v>
       </c>
       <c r="F26">
-        <v>0.3786407766990291</v>
+        <v>0.40625</v>
       </c>
       <c r="G26">
-        <v>0.5100502512562815</v>
+        <v>0.4851851851851852</v>
       </c>
       <c r="H26">
-        <v>0.406</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1076,25 +1076,25 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.5402298850574713</v>
+        <v>0.45</v>
       </c>
       <c r="C27">
-        <v>0.5224550898203593</v>
+        <v>0.5365126676602087</v>
       </c>
       <c r="D27">
-        <v>0.4201680672268908</v>
+        <v>0.42</v>
       </c>
       <c r="E27">
-        <v>0.5090439276485789</v>
+        <v>0.4924433249370277</v>
       </c>
       <c r="F27">
-        <v>0.3853211009174312</v>
+        <v>0.4466019417475728</v>
       </c>
       <c r="G27">
-        <v>0.5075566750629723</v>
+        <v>0.4840686274509804</v>
       </c>
       <c r="H27">
-        <v>0.402</v>
+        <v>0.458</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1102,25 +1102,25 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.5543478260869565</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="C28">
-        <v>0.5225806451612903</v>
+        <v>0.5345821325648416</v>
       </c>
       <c r="D28">
-        <v>0.4107142857142857</v>
+        <v>0.4339622641509434</v>
       </c>
       <c r="E28">
-        <v>0.5134443021766966</v>
+        <v>0.4900249376558604</v>
       </c>
       <c r="F28">
-        <v>0.3981481481481481</v>
+        <v>0.3853211009174312</v>
       </c>
       <c r="G28">
-        <v>0.50187265917603</v>
+        <v>0.4753694581280788</v>
       </c>
       <c r="H28">
-        <v>0.402</v>
+        <v>0.456</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1128,25 +1128,25 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.4952380952380953</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="C29">
-        <v>0.5216480446927374</v>
+        <v>0.5325402379286214</v>
       </c>
       <c r="D29">
-        <v>0.4130434782608696</v>
+        <v>0.5</v>
       </c>
       <c r="E29">
-        <v>0.5</v>
+        <v>0.4867924528301887</v>
       </c>
       <c r="F29">
-        <v>0.4235294117647059</v>
+        <v>0.3894736842105263</v>
       </c>
       <c r="G29">
-        <v>0.5018633540372671</v>
+        <v>0.4732254047322541</v>
       </c>
       <c r="H29">
-        <v>0.392</v>
+        <v>0.446</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1154,25 +1154,25 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.5545454545454546</v>
+        <v>0.5</v>
       </c>
       <c r="C30">
-        <v>0.5217993079584775</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="D30">
-        <v>0.4545454545454545</v>
+        <v>0.46</v>
       </c>
       <c r="E30">
-        <v>0.4911616161616162</v>
+        <v>0.4811557788944724</v>
       </c>
       <c r="F30">
-        <v>0.46875</v>
+        <v>0.4036697247706422</v>
       </c>
       <c r="G30">
-        <v>0.4981504315659679</v>
+        <v>0.4781523096129838</v>
       </c>
       <c r="H30">
-        <v>0.396</v>
+        <v>0.434</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1180,25 +1180,25 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.5565217391304348</v>
+        <v>0.5106382978723404</v>
       </c>
       <c r="C31">
-        <v>0.5167693360711841</v>
+        <v>0.5296864576384256</v>
       </c>
       <c r="D31">
-        <v>0.4426229508196721</v>
+        <v>0.5130434782608696</v>
       </c>
       <c r="E31">
-        <v>0.4860927152317881</v>
+        <v>0.4891994917407878</v>
       </c>
       <c r="F31">
-        <v>0.4787234042553192</v>
+        <v>0.4403669724770642</v>
       </c>
       <c r="G31">
-        <v>0.4987277353689568</v>
+        <v>0.4771573604060914</v>
       </c>
       <c r="H31">
-        <v>0.418</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1206,25 +1206,25 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.5528455284552846</v>
+        <v>0.5638297872340425</v>
       </c>
       <c r="C32">
-        <v>0.5153743315508021</v>
+        <v>0.5328083989501312</v>
       </c>
       <c r="D32">
-        <v>0.4586466165413534</v>
+        <v>0.5315315315315315</v>
       </c>
       <c r="E32">
-        <v>0.4900924702774108</v>
+        <v>0.4869451697127937</v>
       </c>
       <c r="F32">
-        <v>0.5238095238095238</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="G32">
-        <v>0.4925187032418953</v>
+        <v>0.4662420382165605</v>
       </c>
       <c r="H32">
-        <v>0.42</v>
+        <v>0.454</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1232,25 +1232,25 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.5462962962962963</v>
+        <v>0.4905660377358491</v>
       </c>
       <c r="C33">
-        <v>0.5111695137976346</v>
+        <v>0.5297504798464492</v>
       </c>
       <c r="D33">
-        <v>0.4824561403508772</v>
+        <v>0.4516129032258064</v>
       </c>
       <c r="E33">
-        <v>0.4921052631578947</v>
+        <v>0.4830729166666667</v>
       </c>
       <c r="F33">
-        <v>0.5151515151515151</v>
+        <v>0.3673469387755102</v>
       </c>
       <c r="G33">
-        <v>0.4856429463171036</v>
+        <v>0.4769038701622971</v>
       </c>
       <c r="H33">
-        <v>0.432</v>
+        <v>0.436</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1258,25 +1258,25 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.5</v>
+        <v>0.5242718446601942</v>
       </c>
       <c r="C34">
-        <v>0.5167192429022082</v>
+        <v>0.5310913705583756</v>
       </c>
       <c r="D34">
-        <v>0.5663716814159292</v>
+        <v>0.4838709677419355</v>
       </c>
       <c r="E34">
-        <v>0.4923469387755102</v>
+        <v>0.4894179894179894</v>
       </c>
       <c r="F34">
-        <v>0.4907407407407408</v>
+        <v>0.4242424242424243</v>
       </c>
       <c r="G34">
-        <v>0.4907521578298397</v>
+        <v>0.4691046658259773</v>
       </c>
       <c r="H34">
-        <v>0.428</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1284,25 +1284,25 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.5378151260504201</v>
+        <v>0.5089285714285714</v>
       </c>
       <c r="C35">
-        <v>0.5166872682323856</v>
+        <v>0.5291948371235402</v>
       </c>
       <c r="D35">
-        <v>0.46875</v>
+        <v>0.5227272727272727</v>
       </c>
       <c r="E35">
-        <v>0.4912935323383085</v>
+        <v>0.4869109947643979</v>
       </c>
       <c r="F35">
-        <v>0.4895833333333333</v>
+        <v>0.425</v>
       </c>
       <c r="G35">
-        <v>0.4834761321909425</v>
+        <v>0.4668335419274093</v>
       </c>
       <c r="H35">
-        <v>0.436</v>
+        <v>0.424</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1310,25 +1310,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.5555555555555556</v>
+        <v>0.5643564356435643</v>
       </c>
       <c r="C36">
-        <v>0.5147147147147147</v>
+        <v>0.5317365269461077</v>
       </c>
       <c r="D36">
-        <v>0.5051546391752577</v>
+        <v>0.5241935483870968</v>
       </c>
       <c r="E36">
-        <v>0.4969325153374233</v>
+        <v>0.4993581514762516</v>
       </c>
       <c r="F36">
-        <v>0.3846153846153846</v>
+        <v>0.4158415841584158</v>
       </c>
       <c r="G36">
-        <v>0.4854721549636804</v>
+        <v>0.46625</v>
       </c>
       <c r="H36">
-        <v>0.43</v>
+        <v>0.418</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1336,22 +1336,22 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.5321100917431193</v>
+        <v>0.5760869565217391</v>
       </c>
       <c r="C37">
-        <v>0.5126545026486168</v>
+        <v>0.5280833815865663</v>
       </c>
       <c r="D37">
-        <v>0.4591836734693878</v>
+        <v>0.4905660377358491</v>
       </c>
       <c r="E37">
-        <v>0.4974874371859296</v>
+        <v>0.4968314321926489</v>
       </c>
       <c r="F37">
-        <v>0.3974358974358974</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="G37">
-        <v>0.5</v>
+        <v>0.4677222898903776</v>
       </c>
       <c r="H37">
         <v>0.41</v>
@@ -1362,25 +1362,25 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.5689655172413793</v>
+        <v>0.5392156862745098</v>
       </c>
       <c r="C38">
-        <v>0.5109070034443168</v>
+        <v>0.5272931907709623</v>
       </c>
       <c r="D38">
-        <v>0.5</v>
+        <v>0.4888888888888889</v>
       </c>
       <c r="E38">
-        <v>0.5006289308176101</v>
+        <v>0.4968866749688667</v>
       </c>
       <c r="F38">
-        <v>0.375</v>
+        <v>0.3928571428571428</v>
       </c>
       <c r="G38">
-        <v>0.4884287454323995</v>
+        <v>0.4600484261501211</v>
       </c>
       <c r="H38">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1388,25 +1388,25 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.4672897196261682</v>
+        <v>0.5221238938053098</v>
       </c>
       <c r="C39">
-        <v>0.5068181818181818</v>
+        <v>0.5274238227146815</v>
       </c>
       <c r="D39">
-        <v>0.4375</v>
+        <v>0.5111111111111111</v>
       </c>
       <c r="E39">
-        <v>0.5006321112515802</v>
+        <v>0.495049504950495</v>
       </c>
       <c r="F39">
-        <v>0.4193548387096774</v>
+        <v>0.3804347826086957</v>
       </c>
       <c r="G39">
-        <v>0.4956736711990111</v>
+        <v>0.4599514563106796</v>
       </c>
       <c r="H39">
-        <v>0.416</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1414,25 +1414,25 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.5096153846153846</v>
+        <v>0.5051546391752577</v>
       </c>
       <c r="C40">
-        <v>0.5126791620727673</v>
+        <v>0.5301866081229418</v>
       </c>
       <c r="D40">
-        <v>0.4862385321100918</v>
+        <v>0.5213675213675214</v>
       </c>
       <c r="E40">
-        <v>0.5124688279301746</v>
+        <v>0.4880201765447667</v>
       </c>
       <c r="F40">
-        <v>0.4257425742574257</v>
+        <v>0.4673913043478261</v>
       </c>
       <c r="G40">
-        <v>0.4864532019704433</v>
+        <v>0.4618272841051314</v>
       </c>
       <c r="H40">
-        <v>0.42</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1440,25 +1440,25 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.5045045045045045</v>
+        <v>0.5098039215686274</v>
       </c>
       <c r="C41">
-        <v>0.507799892415277</v>
+        <v>0.5261752136752137</v>
       </c>
       <c r="D41">
-        <v>0.54</v>
+        <v>0.5121951219512195</v>
       </c>
       <c r="E41">
-        <v>0.50187265917603</v>
+        <v>0.4883720930232558</v>
       </c>
       <c r="F41">
-        <v>0.4315789473684211</v>
+        <v>0.4406779661016949</v>
       </c>
       <c r="G41">
-        <v>0.4841075794621027</v>
+        <v>0.44472049689441</v>
       </c>
       <c r="H41">
-        <v>0.42</v>
+        <v>0.414</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1466,25 +1466,25 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.4754098360655737</v>
+        <v>0.5252525252525253</v>
       </c>
       <c r="C42">
-        <v>0.5088093966898024</v>
+        <v>0.525130890052356</v>
       </c>
       <c r="D42">
-        <v>0.4854368932038835</v>
+        <v>0.5289256198347108</v>
       </c>
       <c r="E42">
-        <v>0.4987309644670051</v>
+        <v>0.4910485933503836</v>
       </c>
       <c r="F42">
-        <v>0.4888888888888889</v>
+        <v>0.4181818181818182</v>
       </c>
       <c r="G42">
-        <v>0.4794520547945205</v>
+        <v>0.4489281210592686</v>
       </c>
       <c r="H42">
-        <v>0.428</v>
+        <v>0.412</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1492,25 +1492,25 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.543859649122807</v>
+        <v>0.5247524752475248</v>
       </c>
       <c r="C43">
-        <v>0.5097317201472908</v>
+        <v>0.5224948875255624</v>
       </c>
       <c r="D43">
-        <v>0.4758064516129032</v>
+        <v>0.514018691588785</v>
       </c>
       <c r="E43">
-        <v>0.5018963337547409</v>
+        <v>0.4962025316455696</v>
       </c>
       <c r="F43">
-        <v>0.4660194174757282</v>
+        <v>0.4081632653061225</v>
       </c>
       <c r="G43">
-        <v>0.4754299754299754</v>
+        <v>0.4466501240694789</v>
       </c>
       <c r="H43">
-        <v>0.424</v>
+        <v>0.414</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1518,25 +1518,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.5688073394495413</v>
+        <v>0.5471698113207547</v>
       </c>
       <c r="C44">
-        <v>0.502848265147592</v>
+        <v>0.5221327967806841</v>
       </c>
       <c r="D44">
-        <v>0.5046728971962616</v>
+        <v>0.51</v>
       </c>
       <c r="E44">
-        <v>0.4954604409857328</v>
+        <v>0.4974747474747475</v>
       </c>
       <c r="F44">
-        <v>0.5058823529411764</v>
+        <v>0.4320987654320987</v>
       </c>
       <c r="G44">
-        <v>0.4777227722772277</v>
+        <v>0.4419753086419753</v>
       </c>
       <c r="H44">
-        <v>0.416</v>
+        <v>0.412</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1544,25 +1544,25 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.5904761904761905</v>
+        <v>0.5233644859813084</v>
       </c>
       <c r="C45">
-        <v>0.4992389649923896</v>
+        <v>0.5176529090004973</v>
       </c>
       <c r="D45">
-        <v>0.5</v>
+        <v>0.4579439252336449</v>
       </c>
       <c r="E45">
-        <v>0.4885204081632653</v>
+        <v>0.5019108280254777</v>
       </c>
       <c r="F45">
-        <v>0.4897959183673469</v>
+        <v>0.4725274725274725</v>
       </c>
       <c r="G45">
-        <v>0.4707317073170731</v>
+        <v>0.4324324324324325</v>
       </c>
       <c r="H45">
-        <v>0.432</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1570,25 +1570,25 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.5294117647058824</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="C46">
-        <v>0.4932126696832579</v>
+        <v>0.5167652859960552</v>
       </c>
       <c r="D46">
-        <v>0.5431034482758621</v>
+        <v>0.504424778761062</v>
       </c>
       <c r="E46">
-        <v>0.4941935483870968</v>
+        <v>0.5084087968952135</v>
       </c>
       <c r="F46">
-        <v>0.5</v>
+        <v>0.4158415841584158</v>
       </c>
       <c r="G46">
-        <v>0.4719101123595505</v>
+        <v>0.4294631710362047</v>
       </c>
       <c r="H46">
-        <v>0.444</v>
+        <v>0.452</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1596,25 +1596,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.5222222222222223</v>
+        <v>0.5625</v>
       </c>
       <c r="C47">
-        <v>0.5</v>
+        <v>0.5141187925998053</v>
       </c>
       <c r="D47">
-        <v>0.5478260869565217</v>
+        <v>0.4761904761904762</v>
       </c>
       <c r="E47">
-        <v>0.4947643979057592</v>
+        <v>0.507227332457293</v>
       </c>
       <c r="F47">
-        <v>0.449438202247191</v>
+        <v>0.4081632653061225</v>
       </c>
       <c r="G47">
-        <v>0.4775</v>
+        <v>0.4312977099236641</v>
       </c>
       <c r="H47">
-        <v>0.434</v>
+        <v>0.466</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1622,25 +1622,25 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.4943820224719101</v>
+        <v>0.4814814814814815</v>
       </c>
       <c r="C48">
-        <v>0.4990319457889642</v>
+        <v>0.5139423076923076</v>
       </c>
       <c r="D48">
-        <v>0.4491525423728814</v>
+        <v>0.3916666666666667</v>
       </c>
       <c r="E48">
-        <v>0.5051546391752577</v>
+        <v>0.5052770448548812</v>
       </c>
       <c r="F48">
-        <v>0.4285714285714285</v>
+        <v>0.462962962962963</v>
       </c>
       <c r="G48">
-        <v>0.4797047970479705</v>
+        <v>0.4337957124842371</v>
       </c>
       <c r="H48">
-        <v>0.434</v>
+        <v>0.456</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1648,25 +1648,25 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.5125</v>
+        <v>0.4396551724137931</v>
       </c>
       <c r="C49">
-        <v>0.502851711026616</v>
+        <v>0.51725768321513</v>
       </c>
       <c r="D49">
-        <v>0.4956521739130435</v>
+        <v>0.4453781512605042</v>
       </c>
       <c r="E49">
-        <v>0.5128205128205128</v>
+        <v>0.5077922077922078</v>
       </c>
       <c r="F49">
-        <v>0.4019607843137255</v>
+        <v>0.4814814814814815</v>
       </c>
       <c r="G49">
-        <v>0.4806007509386733</v>
+        <v>0.4265822784810127</v>
       </c>
       <c r="H49">
-        <v>0.432</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1674,22 +1674,22 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.5510204081632653</v>
+        <v>0.4297520661157025</v>
       </c>
       <c r="C50">
-        <v>0.5023255813953489</v>
+        <v>0.5178986517898652</v>
       </c>
       <c r="D50">
-        <v>0.456140350877193</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E50">
-        <v>0.514030612244898</v>
+        <v>0.5012820512820513</v>
       </c>
       <c r="F50">
-        <v>0.4479166666666667</v>
+        <v>0.4591836734693878</v>
       </c>
       <c r="G50">
-        <v>0.4800498753117207</v>
+        <v>0.4339152119700748</v>
       </c>
       <c r="H50">
         <v>0.442</v>
@@ -1700,25 +1700,25 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.5490196078431373</v>
+        <v>0.4672131147540984</v>
       </c>
       <c r="C51">
-        <v>0.5020746887966805</v>
+        <v>0.5155677655677655</v>
       </c>
       <c r="D51">
-        <v>0.4912280701754386</v>
+        <v>0.4803921568627451</v>
       </c>
       <c r="E51">
-        <v>0.5121019108280255</v>
+        <v>0.5043914680050188</v>
       </c>
       <c r="F51">
-        <v>0.3978494623655914</v>
+        <v>0.4534883720930232</v>
       </c>
       <c r="G51">
-        <v>0.4687116564417178</v>
+        <v>0.4381067961165049</v>
       </c>
       <c r="H51">
-        <v>0.454</v>
+        <v>0.456</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1726,25 +1726,25 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.5980392156862745</v>
+        <v>0.48</v>
       </c>
       <c r="C52">
-        <v>0.5041133455210237</v>
+        <v>0.5117860380779692</v>
       </c>
       <c r="D52">
-        <v>0.4234234234234234</v>
+        <v>0.5157894736842106</v>
       </c>
       <c r="E52">
-        <v>0.5070967741935484</v>
+        <v>0.4981036662452591</v>
       </c>
       <c r="F52">
-        <v>0.4175824175824176</v>
+        <v>0.3580246913580247</v>
       </c>
       <c r="G52">
-        <v>0.4609665427509294</v>
+        <v>0.4371184371184371</v>
       </c>
       <c r="H52">
-        <v>0.468</v>
+        <v>0.452</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1752,25 +1752,25 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.5</v>
+        <v>0.4406779661016949</v>
       </c>
       <c r="C53">
-        <v>0.5006741573033708</v>
+        <v>0.5115761353517364</v>
       </c>
       <c r="D53">
-        <v>0.3474576271186441</v>
+        <v>0.4700854700854701</v>
       </c>
       <c r="E53">
-        <v>0.5083440308087291</v>
+        <v>0.4956085319949812</v>
       </c>
       <c r="F53">
-        <v>0.4903846153846154</v>
+        <v>0.4606741573033708</v>
       </c>
       <c r="G53">
-        <v>0.4554455445544555</v>
+        <v>0.4432234432234432</v>
       </c>
       <c r="H53">
-        <v>0.474</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1778,25 +1778,25 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.5268817204301075</v>
+        <v>0.4453781512605042</v>
       </c>
       <c r="C54">
-        <v>0.5059813912272929</v>
+        <v>0.5134782608695653</v>
       </c>
       <c r="D54">
-        <v>0.4077669902912621</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="E54">
-        <v>0.5032175032175032</v>
+        <v>0.5037783375314862</v>
       </c>
       <c r="F54">
-        <v>0.5154639175257731</v>
+        <v>0.4742268041237113</v>
       </c>
       <c r="G54">
-        <v>0.4508094645080947</v>
+        <v>0.4384057971014493</v>
       </c>
       <c r="H54">
-        <v>0.472</v>
+        <v>0.446</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1804,25 +1804,25 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.5137614678899083</v>
+        <v>0.4857142857142857</v>
       </c>
       <c r="C55">
-        <v>0.504110774556469</v>
+        <v>0.5148259561667383</v>
       </c>
       <c r="D55">
-        <v>0.4385964912280702</v>
+        <v>0.4807692307692308</v>
       </c>
       <c r="E55">
-        <v>0.4937655860349127</v>
+        <v>0.5</v>
       </c>
       <c r="F55">
-        <v>0.5263157894736842</v>
+        <v>0.4021739130434783</v>
       </c>
       <c r="G55">
-        <v>0.4554334554334554</v>
+        <v>0.4396551724137931</v>
       </c>
       <c r="H55">
-        <v>0.466</v>
+        <v>0.434</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1830,25 +1830,25 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.5420560747663551</v>
+        <v>0.4476190476190476</v>
       </c>
       <c r="C56">
-        <v>0.5051502145922747</v>
+        <v>0.5109612141652614</v>
       </c>
       <c r="D56">
-        <v>0.4339622641509434</v>
+        <v>0.3839285714285715</v>
       </c>
       <c r="E56">
-        <v>0.4836683417085427</v>
+        <v>0.5031928480204342</v>
       </c>
       <c r="F56">
-        <v>0.5056179775280899</v>
+        <v>0.4479166666666667</v>
       </c>
       <c r="G56">
-        <v>0.4658536585365854</v>
+        <v>0.4578163771712159</v>
       </c>
       <c r="H56">
-        <v>0.454</v>
+        <v>0.408</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1856,25 +1856,25 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.4741379310344828</v>
+        <v>0.4537037037037037</v>
       </c>
       <c r="C57">
-        <v>0.5023295213892418</v>
+        <v>0.5150880134115675</v>
       </c>
       <c r="D57">
-        <v>0.4504504504504505</v>
+        <v>0.3928571428571428</v>
       </c>
       <c r="E57">
-        <v>0.4816223067173637</v>
+        <v>0.5086321381142098</v>
       </c>
       <c r="F57">
-        <v>0.4782608695652174</v>
+        <v>0.4554455445544555</v>
       </c>
       <c r="G57">
-        <v>0.4766584766584767</v>
+        <v>0.4572158365261814</v>
       </c>
       <c r="H57">
-        <v>0.446</v>
+        <v>0.406</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1882,25 +1882,25 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.4576271186440678</v>
+        <v>0.4742268041237113</v>
       </c>
       <c r="C58">
-        <v>0.5043877977434184</v>
+        <v>0.5150391429748661</v>
       </c>
       <c r="D58">
-        <v>0.5</v>
+        <v>0.3834586466165413</v>
       </c>
       <c r="E58">
-        <v>0.4848101265822785</v>
+        <v>0.5123537061118335</v>
       </c>
       <c r="F58">
-        <v>0.4787234042553192</v>
+        <v>0.464</v>
       </c>
       <c r="G58">
-        <v>0.4852941176470588</v>
+        <v>0.4562737642585551</v>
       </c>
       <c r="H58">
-        <v>0.442</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1908,25 +1908,25 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.4587155963302753</v>
+        <v>0.4454545454545454</v>
       </c>
       <c r="C59">
-        <v>0.5039110745162618</v>
+        <v>0.5122934300685208</v>
       </c>
       <c r="D59">
-        <v>0.5142857142857142</v>
+        <v>0.4086956521739131</v>
       </c>
       <c r="E59">
-        <v>0.4807930607187113</v>
+        <v>0.5038461538461538</v>
       </c>
       <c r="F59">
-        <v>0.3617021276595745</v>
+        <v>0.4636363636363636</v>
       </c>
       <c r="G59">
-        <v>0.4811664641555286</v>
+        <v>0.4578616352201258</v>
       </c>
       <c r="H59">
-        <v>0.444</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1934,25 +1934,25 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.4455445544554456</v>
+        <v>0.4766355140186916</v>
       </c>
       <c r="C60">
-        <v>0.5008103727714749</v>
+        <v>0.5155378486055777</v>
       </c>
       <c r="D60">
-        <v>0.4767441860465116</v>
+        <v>0.4074074074074074</v>
       </c>
       <c r="E60">
-        <v>0.4761306532663316</v>
+        <v>0.493734335839599</v>
       </c>
       <c r="F60">
-        <v>0.3595505617977528</v>
+        <v>0.4639175257731959</v>
       </c>
       <c r="G60">
-        <v>0.4852579852579852</v>
+        <v>0.4477244772447724</v>
       </c>
       <c r="H60">
-        <v>0.456</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1960,25 +1960,25 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.4659090909090909</v>
+        <v>0.4090909090909091</v>
       </c>
       <c r="C61">
-        <v>0.5013894402540691</v>
+        <v>0.5117831893165751</v>
       </c>
       <c r="D61">
-        <v>0.5188679245283019</v>
+        <v>0.3904761904761905</v>
       </c>
       <c r="E61">
-        <v>0.474009900990099</v>
+        <v>0.491183879093199</v>
       </c>
       <c r="F61">
-        <v>0.3979591836734694</v>
+        <v>0.4375</v>
       </c>
       <c r="G61">
-        <v>0.4815724815724816</v>
+        <v>0.454656862745098</v>
       </c>
       <c r="H61">
-        <v>0.456</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1986,25 +1986,25 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.4854368932038835</v>
+        <v>0.4054054054054054</v>
       </c>
       <c r="C62">
-        <v>0.4970599764798118</v>
+        <v>0.5171473109898675</v>
       </c>
       <c r="D62">
-        <v>0.5263157894736842</v>
+        <v>0.4144144144144144</v>
       </c>
       <c r="E62">
-        <v>0.4833759590792839</v>
+        <v>0.4762516046213094</v>
       </c>
       <c r="F62">
-        <v>0.4736842105263158</v>
+        <v>0.4489795918367347</v>
       </c>
       <c r="G62">
-        <v>0.4837092731829574</v>
+        <v>0.4543178973717146</v>
       </c>
       <c r="H62">
-        <v>0.46</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2012,25 +2012,25 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.5208333333333334</v>
+        <v>0.3831775700934579</v>
       </c>
       <c r="C63">
-        <v>0.4943557804593227</v>
+        <v>0.515793528505393</v>
       </c>
       <c r="D63">
-        <v>0.5740740740740741</v>
+        <v>0.336283185840708</v>
       </c>
       <c r="E63">
-        <v>0.4847715736040609</v>
+        <v>0.4807692307692308</v>
       </c>
       <c r="F63">
-        <v>0.4230769230769231</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="G63">
-        <v>0.4730238393977415</v>
+        <v>0.4600997506234414</v>
       </c>
       <c r="H63">
-        <v>0.454</v>
+        <v>0.396</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2038,25 +2038,25 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.4607843137254902</v>
+        <v>0.4245283018867925</v>
       </c>
       <c r="C64">
-        <v>0.4934815950920245</v>
+        <v>0.5165336374002281</v>
       </c>
       <c r="D64">
-        <v>0.509090909090909</v>
+        <v>0.4509803921568628</v>
       </c>
       <c r="E64">
-        <v>0.4923076923076923</v>
+        <v>0.4904214559386973</v>
       </c>
       <c r="F64">
-        <v>0.4259259259259259</v>
+        <v>0.48</v>
       </c>
       <c r="G64">
-        <v>0.4736180904522613</v>
+        <v>0.4590570719602978</v>
       </c>
       <c r="H64">
-        <v>0.442</v>
+        <v>0.408</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2064,25 +2064,25 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.504424778761062</v>
+        <v>0.4433962264150944</v>
       </c>
       <c r="C65">
-        <v>0.4971601666035593</v>
+        <v>0.5123688155922039</v>
       </c>
       <c r="D65">
-        <v>0.4666666666666667</v>
+        <v>0.4770642201834863</v>
       </c>
       <c r="E65">
-        <v>0.5057766367137355</v>
+        <v>0.4829760403530896</v>
       </c>
       <c r="F65">
-        <v>0.4196428571428572</v>
+        <v>0.3695652173913043</v>
       </c>
       <c r="G65">
-        <v>0.4715549936788875</v>
+        <v>0.4610630407911001</v>
       </c>
       <c r="H65">
-        <v>0.442</v>
+        <v>0.422</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2090,25 +2090,25 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.4959349593495935</v>
+        <v>0.4761904761904762</v>
       </c>
       <c r="C66">
-        <v>0.4938317757009346</v>
+        <v>0.5107407407407407</v>
       </c>
       <c r="D66">
-        <v>0.4299065420560748</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="E66">
-        <v>0.5050125313283208</v>
+        <v>0.4831038798498123</v>
       </c>
       <c r="F66">
-        <v>0.495049504950495</v>
+        <v>0.34375</v>
       </c>
       <c r="G66">
-        <v>0.4625</v>
+        <v>0.4702308626974483</v>
       </c>
       <c r="H66">
-        <v>0.44</v>
+        <v>0.422</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2116,25 +2116,25 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.4528301886792453</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="C67">
-        <v>0.493125232255667</v>
+        <v>0.5111598975484816</v>
       </c>
       <c r="D67">
-        <v>0.4607843137254902</v>
+        <v>0.4693877551020408</v>
       </c>
       <c r="E67">
-        <v>0.4993710691823899</v>
+        <v>0.4832298136645963</v>
       </c>
       <c r="F67">
-        <v>0.5</v>
+        <v>0.3804347826086957</v>
       </c>
       <c r="G67">
-        <v>0.4533169533169533</v>
+        <v>0.4621026894865526</v>
       </c>
       <c r="H67">
-        <v>0.44</v>
+        <v>0.422</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2142,25 +2142,25 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.4479166666666667</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="C68">
-        <v>0.4965290464011692</v>
+        <v>0.50920245398773</v>
       </c>
       <c r="D68">
-        <v>0.4528301886792453</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="E68">
-        <v>0.4910941475826972</v>
+        <v>0.4801488833746898</v>
       </c>
       <c r="F68">
-        <v>0.5053763440860215</v>
+        <v>0.4395604395604396</v>
       </c>
       <c r="G68">
-        <v>0.4612546125461255</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="H68">
-        <v>0.438</v>
+        <v>0.422</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2168,25 +2168,25 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.47</v>
+        <v>0.4766355140186916</v>
       </c>
       <c r="C69">
-        <v>0.4967672413793103</v>
+        <v>0.5112379593292901</v>
       </c>
       <c r="D69">
-        <v>0.4827586206896552</v>
+        <v>0.4574468085106383</v>
       </c>
       <c r="E69">
-        <v>0.4955863808322825</v>
+        <v>0.4810744810744811</v>
       </c>
       <c r="F69">
-        <v>0.4954128440366973</v>
+        <v>0.4845360824742268</v>
       </c>
       <c r="G69">
-        <v>0.4699386503067485</v>
+        <v>0.4539951573849879</v>
       </c>
       <c r="H69">
-        <v>0.43</v>
+        <v>0.426</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2194,25 +2194,25 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.5188679245283019</v>
+        <v>0.4414414414414414</v>
       </c>
       <c r="C70">
-        <v>0.4959378311550689</v>
+        <v>0.5126849894291755</v>
       </c>
       <c r="D70">
-        <v>0.3958333333333333</v>
+        <v>0.4835164835164835</v>
       </c>
       <c r="E70">
-        <v>0.4956195244055069</v>
+        <v>0.4888613861386139</v>
       </c>
       <c r="F70">
-        <v>0.5288461538461539</v>
+        <v>0.4634146341463415</v>
       </c>
       <c r="G70">
-        <v>0.4766009852216749</v>
+        <v>0.4574599260172627</v>
       </c>
       <c r="H70">
-        <v>0.416</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2220,25 +2220,25 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.543859649122807</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="C71">
-        <v>0.4971969166082691</v>
+        <v>0.5129009762900977</v>
       </c>
       <c r="D71">
-        <v>0.3684210526315789</v>
+        <v>0.4387755102040816</v>
       </c>
       <c r="E71">
-        <v>0.4943960149439601</v>
+        <v>0.4868585732165207</v>
       </c>
       <c r="F71">
-        <v>0.4347826086956522</v>
+        <v>0.4148936170212766</v>
       </c>
       <c r="G71">
-        <v>0.4594257178526842</v>
+        <v>0.463980463980464</v>
       </c>
       <c r="H71">
-        <v>0.444</v>
+        <v>0.404</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2246,25 +2246,25 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.5398230088495575</v>
+        <v>0.4910714285714285</v>
       </c>
       <c r="C72">
-        <v>0.4973840251133589</v>
+        <v>0.5131034482758621</v>
       </c>
       <c r="D72">
-        <v>0.3539823008849557</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="E72">
-        <v>0.4942233632862644</v>
+        <v>0.4892268694550063</v>
       </c>
       <c r="F72">
-        <v>0.5339805825242718</v>
+        <v>0.3775510204081632</v>
       </c>
       <c r="G72">
-        <v>0.4700636942675159</v>
+        <v>0.4594257178526842</v>
       </c>
       <c r="H72">
-        <v>0.432</v>
+        <v>0.412</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2272,25 +2272,25 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.5045871559633027</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="C73">
-        <v>0.4979296066252588</v>
+        <v>0.5134766291368134</v>
       </c>
       <c r="D73">
-        <v>0.3888888888888889</v>
+        <v>0.4571428571428571</v>
       </c>
       <c r="E73">
-        <v>0.4928104575163399</v>
+        <v>0.4835443037974684</v>
       </c>
       <c r="F73">
-        <v>0.5454545454545454</v>
+        <v>0.4257425742574257</v>
       </c>
       <c r="G73">
-        <v>0.4704370179948586</v>
+        <v>0.4632627646326277</v>
       </c>
       <c r="H73">
-        <v>0.434</v>
+        <v>0.418</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2298,25 +2298,25 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.4905660377358491</v>
+        <v>0.5327868852459017</v>
       </c>
       <c r="C74">
-        <v>0.4998297582567245</v>
+        <v>0.5143726750084545</v>
       </c>
       <c r="D74">
-        <v>0.4188034188034188</v>
+        <v>0.4090909090909091</v>
       </c>
       <c r="E74">
-        <v>0.4856396866840731</v>
+        <v>0.484197218710493</v>
       </c>
       <c r="F74">
-        <v>0.4869565217391305</v>
+        <v>0.4683544303797468</v>
       </c>
       <c r="G74">
-        <v>0.4781491002570694</v>
+        <v>0.4611590628853268</v>
       </c>
       <c r="H74">
-        <v>0.434</v>
+        <v>0.406</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2324,25 +2324,25 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.5145631067961165</v>
+        <v>0.4424778761061947</v>
       </c>
       <c r="C75">
-        <v>0.5005048805116122</v>
+        <v>0.5108950720750922</v>
       </c>
       <c r="D75">
-        <v>0.4247787610619469</v>
+        <v>0.4260869565217391</v>
       </c>
       <c r="E75">
-        <v>0.4839948783610755</v>
+        <v>0.4942675159235669</v>
       </c>
       <c r="F75">
-        <v>0.4956521739130435</v>
+        <v>0.4659090909090909</v>
       </c>
       <c r="G75">
-        <v>0.4949367088607595</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="H75">
-        <v>0.43</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2350,25 +2350,25 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.5045045045045045</v>
+        <v>0.452991452991453</v>
       </c>
       <c r="C76">
-        <v>0.50066401062417</v>
+        <v>0.512396694214876</v>
       </c>
       <c r="D76">
-        <v>0.3644859813084112</v>
+        <v>0.4018691588785047</v>
       </c>
       <c r="E76">
-        <v>0.4766118836915297</v>
+        <v>0.4949238578680203</v>
       </c>
       <c r="F76">
-        <v>0.4310344827586207</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="G76">
-        <v>0.490613266583229</v>
+        <v>0.4664224664224664</v>
       </c>
       <c r="H76">
-        <v>0.428</v>
+        <v>0.394</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2379,22 +2379,22 @@
         <v>0.5344827586206896</v>
       </c>
       <c r="C77">
-        <v>0.4995047870584352</v>
+        <v>0.512753433616743</v>
       </c>
       <c r="D77">
-        <v>0.3608247422680412</v>
+        <v>0.4893617021276596</v>
       </c>
       <c r="E77">
-        <v>0.4808673469387755</v>
+        <v>0.5012468827930174</v>
       </c>
       <c r="F77">
-        <v>0.3723404255319149</v>
+        <v>0.4269662921348314</v>
       </c>
       <c r="G77">
-        <v>0.4987309644670051</v>
+        <v>0.4660194174757282</v>
       </c>
       <c r="H77">
-        <v>0.422</v>
+        <v>0.396</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2402,25 +2402,25 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.5283018867924528</v>
+        <v>0.5514018691588785</v>
       </c>
       <c r="C78">
-        <v>0.4949163660216465</v>
+        <v>0.5055087491898899</v>
       </c>
       <c r="D78">
-        <v>0.4770642201834863</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="E78">
-        <v>0.4834183673469388</v>
+        <v>0.4907063197026023</v>
       </c>
       <c r="F78">
-        <v>0.4105263157894737</v>
+        <v>0.4</v>
       </c>
       <c r="G78">
-        <v>0.5050251256281407</v>
+        <v>0.4694376528117359</v>
       </c>
       <c r="H78">
-        <v>0.43</v>
+        <v>0.392</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2428,25 +2428,25 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.4851485148514851</v>
+        <v>0.49</v>
       </c>
       <c r="C79">
-        <v>0.4970986460348162</v>
+        <v>0.5057618437900128</v>
       </c>
       <c r="D79">
-        <v>0.5</v>
+        <v>0.5108695652173914</v>
       </c>
       <c r="E79">
-        <v>0.4691823899371069</v>
+        <v>0.4869888475836431</v>
       </c>
       <c r="F79">
-        <v>0.375</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="G79">
-        <v>0.4963235294117647</v>
+        <v>0.4734895191122072</v>
       </c>
       <c r="H79">
-        <v>0.432</v>
+        <v>0.398</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2454,25 +2454,25 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.4770642201834863</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="C80">
-        <v>0.5011178537208559</v>
+        <v>0.5069974554707379</v>
       </c>
       <c r="D80">
-        <v>0.3980582524271845</v>
+        <v>0.4554455445544555</v>
       </c>
       <c r="E80">
-        <v>0.4820512820512821</v>
+        <v>0.4924050632911393</v>
       </c>
       <c r="F80">
-        <v>0.4444444444444444</v>
+        <v>0.4571428571428571</v>
       </c>
       <c r="G80">
-        <v>0.4900249376558604</v>
+        <v>0.4774436090225564</v>
       </c>
       <c r="H80">
-        <v>0.438</v>
+        <v>0.392</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2480,25 +2480,25 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0.4310344827586207</v>
+        <v>0.5096153846153846</v>
       </c>
       <c r="C81">
-        <v>0.5022068095838588</v>
+        <v>0.5085551330798479</v>
       </c>
       <c r="D81">
-        <v>0.4070796460176991</v>
+        <v>0.4786324786324787</v>
       </c>
       <c r="E81">
-        <v>0.4804539722572509</v>
+        <v>0.4934895833333333</v>
       </c>
       <c r="F81">
-        <v>0.3232323232323233</v>
+        <v>0.4077669902912621</v>
       </c>
       <c r="G81">
-        <v>0.4815724815724816</v>
+        <v>0.4665809768637532</v>
       </c>
       <c r="H81">
-        <v>0.438</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2506,25 +2506,25 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.4473684210526316</v>
+        <v>0.5408163265306123</v>
       </c>
       <c r="C82">
-        <v>0.5034547738693468</v>
+        <v>0.5061071093015972</v>
       </c>
       <c r="D82">
-        <v>0.3820224719101123</v>
+        <v>0.46875</v>
       </c>
       <c r="E82">
-        <v>0.4719387755102041</v>
+        <v>0.4897959183673469</v>
       </c>
       <c r="F82">
-        <v>0.4021739130434783</v>
+        <v>0.4363636363636363</v>
       </c>
       <c r="G82">
-        <v>0.4776674937965261</v>
+        <v>0.4676616915422885</v>
       </c>
       <c r="H82">
-        <v>0.446</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2532,25 +2532,25 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0.4587155963302753</v>
+        <v>0.5370370370370371</v>
       </c>
       <c r="C83">
-        <v>0.5026422132421511</v>
+        <v>0.5043130006161429</v>
       </c>
       <c r="D83">
-        <v>0.4336283185840708</v>
+        <v>0.4842105263157895</v>
       </c>
       <c r="E83">
-        <v>0.4756554307116105</v>
+        <v>0.4880803011292346</v>
       </c>
       <c r="F83">
-        <v>0.4035087719298245</v>
+        <v>0.4941176470588236</v>
       </c>
       <c r="G83">
-        <v>0.4684796044499382</v>
+        <v>0.4574209245742092</v>
       </c>
       <c r="H83">
-        <v>0.452</v>
+        <v>0.442</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2558,25 +2558,25 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0.4910714285714285</v>
+        <v>0.4954128440366973</v>
       </c>
       <c r="C84">
-        <v>0.5032377428307123</v>
+        <v>0.503671970624235</v>
       </c>
       <c r="D84">
-        <v>0.4285714285714285</v>
+        <v>0.5180722891566265</v>
       </c>
       <c r="E84">
-        <v>0.4719387755102041</v>
+        <v>0.4920245398773006</v>
       </c>
       <c r="F84">
-        <v>0.3571428571428572</v>
+        <v>0.4177215189873418</v>
       </c>
       <c r="G84">
-        <v>0.4748110831234257</v>
+        <v>0.4483173076923077</v>
       </c>
       <c r="H84">
-        <v>0.446</v>
+        <v>0.444</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2584,25 +2584,25 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0.5128205128205128</v>
+        <v>0.4845360824742268</v>
       </c>
       <c r="C85">
-        <v>0.5016845329249617</v>
+        <v>0.505624809972636</v>
       </c>
       <c r="D85">
-        <v>0.4173913043478261</v>
+        <v>0.5287356321839081</v>
       </c>
       <c r="E85">
-        <v>0.4797979797979798</v>
+        <v>0.4863861386138614</v>
       </c>
       <c r="F85">
-        <v>0.38</v>
+        <v>0.4395604395604396</v>
       </c>
       <c r="G85">
-        <v>0.4745972738537794</v>
+        <v>0.4486552567237164</v>
       </c>
       <c r="H85">
-        <v>0.436</v>
+        <v>0.452</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2610,25 +2610,25 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0.5480769230769231</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="C86">
-        <v>0.5027422303473492</v>
+        <v>0.5050898203592814</v>
       </c>
       <c r="D86">
-        <v>0.4363636363636363</v>
+        <v>0.5</v>
       </c>
       <c r="E86">
-        <v>0.4808184143222506</v>
+        <v>0.4827586206896552</v>
       </c>
       <c r="F86">
-        <v>0.3372093023255814</v>
+        <v>0.4711538461538461</v>
       </c>
       <c r="G86">
-        <v>0.4770186335403727</v>
+        <v>0.4403444034440344</v>
       </c>
       <c r="H86">
-        <v>0.446</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2636,25 +2636,25 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.5196078431372549</v>
+        <v>0.4954954954954955</v>
       </c>
       <c r="C87">
-        <v>0.5009030704394943</v>
+        <v>0.5029585798816568</v>
       </c>
       <c r="D87">
-        <v>0.4054054054054054</v>
+        <v>0.45</v>
       </c>
       <c r="E87">
-        <v>0.4774193548387097</v>
+        <v>0.4773299748110831</v>
       </c>
       <c r="F87">
-        <v>0.3863636363636364</v>
+        <v>0.4482758620689655</v>
       </c>
       <c r="G87">
-        <v>0.4715346534653465</v>
+        <v>0.4451294697903823</v>
       </c>
       <c r="H87">
-        <v>0.44</v>
+        <v>0.464</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2662,25 +2662,25 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.5729166666666666</v>
+        <v>0.5585585585585585</v>
       </c>
       <c r="C88">
-        <v>0.5016315633343221</v>
+        <v>0.503985828166519</v>
       </c>
       <c r="D88">
-        <v>0.4661016949152542</v>
+        <v>0.422680412371134</v>
       </c>
       <c r="E88">
-        <v>0.4811557788944724</v>
+        <v>0.4905660377358491</v>
       </c>
       <c r="F88">
-        <v>0.4123711340206185</v>
+        <v>0.4946236559139785</v>
       </c>
       <c r="G88">
-        <v>0.463768115942029</v>
+        <v>0.4607843137254902</v>
       </c>
       <c r="H88">
-        <v>0.442</v>
+        <v>0.456</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2688,25 +2688,25 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.4565217391304348</v>
+        <v>0.4873949579831933</v>
       </c>
       <c r="C89">
-        <v>0.4991212653778559</v>
+        <v>0.5024875621890548</v>
       </c>
       <c r="D89">
-        <v>0.4545454545454545</v>
+        <v>0.4424778761061947</v>
       </c>
       <c r="E89">
-        <v>0.4800498753117207</v>
+        <v>0.4987437185929648</v>
       </c>
       <c r="F89">
-        <v>0.4025974025974026</v>
+        <v>0.4536082474226804</v>
       </c>
       <c r="G89">
-        <v>0.4547647768395657</v>
+        <v>0.4611590628853268</v>
       </c>
       <c r="H89">
-        <v>0.446</v>
+        <v>0.458</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2714,25 +2714,25 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.5104166666666666</v>
+        <v>0.5210084033613446</v>
       </c>
       <c r="C90">
-        <v>0.5002906976744186</v>
+        <v>0.5056735525167297</v>
       </c>
       <c r="D90">
-        <v>0.4893617021276596</v>
+        <v>0.4622641509433962</v>
       </c>
       <c r="E90">
-        <v>0.4850374064837905</v>
+        <v>0.5006337135614702</v>
       </c>
       <c r="F90">
-        <v>0.375</v>
+        <v>0.42</v>
       </c>
       <c r="G90">
-        <v>0.4512635379061372</v>
+        <v>0.4631449631449631</v>
       </c>
       <c r="H90">
-        <v>0.438</v>
+        <v>0.444</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2740,25 +2740,25 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.52</v>
+        <v>0.6033057851239669</v>
       </c>
       <c r="C91">
-        <v>0.4978404837316441</v>
+        <v>0.5015946651203247</v>
       </c>
       <c r="D91">
-        <v>0.5247524752475248</v>
+        <v>0.4134615384615384</v>
       </c>
       <c r="E91">
-        <v>0.4801488833746898</v>
+        <v>0.4923469387755102</v>
       </c>
       <c r="F91">
-        <v>0.4269662921348314</v>
+        <v>0.3854166666666667</v>
       </c>
       <c r="G91">
-        <v>0.4594921402660218</v>
+        <v>0.4680050188205772</v>
       </c>
       <c r="H91">
-        <v>0.436</v>
+        <v>0.434</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2766,25 +2766,25 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.5132743362831859</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="C92">
-        <v>0.498282770463652</v>
+        <v>0.4981316470250072</v>
       </c>
       <c r="D92">
-        <v>0.4242424242424243</v>
+        <v>0.5130434782608696</v>
       </c>
       <c r="E92">
-        <v>0.4860406091370558</v>
+        <v>0.4943253467843632</v>
       </c>
       <c r="F92">
-        <v>0.4631578947368421</v>
+        <v>0.4563106796116505</v>
       </c>
       <c r="G92">
-        <v>0.4573547589616811</v>
+        <v>0.4654320987654321</v>
       </c>
       <c r="H92">
-        <v>0.426</v>
+        <v>0.436</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2792,25 +2792,25 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.5327102803738317</v>
+        <v>0.5925925925925926</v>
       </c>
       <c r="C93">
-        <v>0.4968732234223991</v>
+        <v>0.4994295493439818</v>
       </c>
       <c r="D93">
-        <v>0.4594594594594595</v>
+        <v>0.4368932038834951</v>
       </c>
       <c r="E93">
-        <v>0.4968152866242038</v>
+        <v>0.4891994917407878</v>
       </c>
       <c r="F93">
-        <v>0.4150943396226415</v>
+        <v>0.3809523809523809</v>
       </c>
       <c r="G93">
-        <v>0.45875</v>
+        <v>0.4716049382716049</v>
       </c>
       <c r="H93">
-        <v>0.428</v>
+        <v>0.414</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2818,25 +2818,25 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.5283018867924528</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="C94">
-        <v>0.4953664700926706</v>
+        <v>0.4981653965565905</v>
       </c>
       <c r="D94">
-        <v>0.4811320754716981</v>
+        <v>0.4313725490196079</v>
       </c>
       <c r="E94">
-        <v>0.4912280701754386</v>
+        <v>0.4993646759847522</v>
       </c>
       <c r="F94">
-        <v>0.4</v>
+        <v>0.4215686274509804</v>
       </c>
       <c r="G94">
-        <v>0.4530864197530864</v>
+        <v>0.4797546012269939</v>
       </c>
       <c r="H94">
-        <v>0.434</v>
+        <v>0.408</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2844,25 +2844,25 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.5238095238095238</v>
+        <v>0.5283018867924528</v>
       </c>
       <c r="C95">
-        <v>0.4955431754874652</v>
+        <v>0.4994397759103641</v>
       </c>
       <c r="D95">
-        <v>0.4565217391304348</v>
+        <v>0.4036697247706422</v>
       </c>
       <c r="E95">
-        <v>0.4968789013732834</v>
+        <v>0.4892541087231353</v>
       </c>
       <c r="F95">
-        <v>0.4606741573033708</v>
+        <v>0.4242424242424243</v>
       </c>
       <c r="G95">
-        <v>0.4600484261501211</v>
+        <v>0.472636815920398</v>
       </c>
       <c r="H95">
-        <v>0.422</v>
+        <v>0.416</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2870,25 +2870,25 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.5370370370370371</v>
+        <v>0.509090909090909</v>
       </c>
       <c r="C96">
-        <v>0.4950221238938053</v>
+        <v>0.4986103390772652</v>
       </c>
       <c r="D96">
-        <v>0.4693877551020408</v>
+        <v>0.4038461538461539</v>
       </c>
       <c r="E96">
-        <v>0.493167701863354</v>
+        <v>0.4974619289340101</v>
       </c>
       <c r="F96">
-        <v>0.3478260869565217</v>
+        <v>0.4301075268817204</v>
       </c>
       <c r="G96">
-        <v>0.4574209245742092</v>
+        <v>0.4727722772277227</v>
       </c>
       <c r="H96">
-        <v>0.422</v>
+        <v>0.416</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2896,25 +2896,25 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.5346534653465347</v>
+        <v>0.5327102803738317</v>
       </c>
       <c r="C97">
-        <v>0.493969298245614</v>
+        <v>0.5002748763056625</v>
       </c>
       <c r="D97">
-        <v>0.5157894736842106</v>
+        <v>0.4299065420560748</v>
       </c>
       <c r="E97">
-        <v>0.4871165644171779</v>
+        <v>0.4943960149439601</v>
       </c>
       <c r="F97">
-        <v>0.4020618556701031</v>
+        <v>0.4141414141414141</v>
       </c>
       <c r="G97">
-        <v>0.4664268585131894</v>
+        <v>0.4732360097323601</v>
       </c>
       <c r="H97">
-        <v>0.422</v>
+        <v>0.406</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2922,25 +2922,25 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0.5339805825242718</v>
+        <v>0.5648148148148148</v>
       </c>
       <c r="C98">
-        <v>0.4955102040816327</v>
+        <v>0.4995900519267559</v>
       </c>
       <c r="D98">
-        <v>0.5222222222222223</v>
+        <v>0.38</v>
       </c>
       <c r="E98">
-        <v>0.4815724815724816</v>
+        <v>0.4924433249370277</v>
       </c>
       <c r="F98">
-        <v>0.4146341463414634</v>
+        <v>0.4175824175824176</v>
       </c>
       <c r="G98">
-        <v>0.4671532846715328</v>
+        <v>0.4734895191122072</v>
       </c>
       <c r="H98">
-        <v>0.424</v>
+        <v>0.414</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2948,25 +2948,25 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0.4854368932038835</v>
+        <v>0.5225225225225225</v>
       </c>
       <c r="C99">
-        <v>0.4952689916193566</v>
+        <v>0.499184339314845</v>
       </c>
       <c r="D99">
-        <v>0.4536082474226804</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="E99">
-        <v>0.4717444717444718</v>
+        <v>0.4897959183673469</v>
       </c>
       <c r="F99">
-        <v>0.4680851063829787</v>
+        <v>0.3936170212765958</v>
       </c>
       <c r="G99">
-        <v>0.4681107099879663</v>
+        <v>0.4701492537313433</v>
       </c>
       <c r="H99">
-        <v>0.414</v>
+        <v>0.418</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2974,25 +2974,25 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0.4736842105263158</v>
+        <v>0.5178571428571429</v>
       </c>
       <c r="C100">
-        <v>0.4970366379310345</v>
+        <v>0.4994600431965443</v>
       </c>
       <c r="D100">
-        <v>0.4631578947368421</v>
+        <v>0.3983050847457627</v>
       </c>
       <c r="E100">
-        <v>0.471105527638191</v>
+        <v>0.4846938775510204</v>
       </c>
       <c r="F100">
-        <v>0.4945054945054945</v>
+        <v>0.4421052631578947</v>
       </c>
       <c r="G100">
-        <v>0.4592592592592593</v>
+        <v>0.4684014869888476</v>
       </c>
       <c r="H100">
-        <v>0.422</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -3000,25 +3000,25 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0.4553571428571428</v>
+        <v>0.4608695652173913</v>
       </c>
       <c r="C101">
-        <v>0.4970445996775927</v>
+        <v>0.500534188034188</v>
       </c>
       <c r="D101">
-        <v>0.4347826086956522</v>
+        <v>0.4864864864864865</v>
       </c>
       <c r="E101">
-        <v>0.469309462915601</v>
+        <v>0.4816223067173637</v>
       </c>
       <c r="F101">
-        <v>0.4953271028037383</v>
+        <v>0.4842105263157895</v>
       </c>
       <c r="G101">
-        <v>0.4522613065326633</v>
+        <v>0.4669926650366748</v>
       </c>
       <c r="H101">
-        <v>0.434</v>
+        <v>0.408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>